<commit_message>
-- ResponseBuffering=adaptive is used --Added OracleClients with Details of problem statement
</commit_message>
<xml_diff>
--- a/reports/Opera-Client-Streaming-Measurements.xlsx
+++ b/reports/Opera-Client-Streaming-Measurements.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\idnakj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\OperaClientStreaming\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="4890" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="4890"/>
   </bookViews>
   <sheets>
     <sheet name="1 StreamingSources" sheetId="12" r:id="rId1"/>
@@ -17,10 +17,8 @@
     <sheet name="3 StreamingSources" sheetId="3" r:id="rId3"/>
     <sheet name="4 StreamingSources" sheetId="4" r:id="rId4"/>
     <sheet name="5 StreamingSources" sheetId="5" r:id="rId5"/>
+    <sheet name="2000K-MultipleSources" sheetId="13" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId6"/>
-  </externalReferences>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -31,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="32">
   <si>
     <t>"-Xmx512m"</t>
   </si>
@@ -119,6 +117,15 @@
   <si>
     <t>OOM issue</t>
   </si>
+  <si>
+    <t>No of Sources</t>
+  </si>
+  <si>
+    <t>Time (secs)</t>
+  </si>
+  <si>
+    <t>OOM</t>
+  </si>
 </sst>
 </file>
 
@@ -159,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -182,11 +189,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -200,6 +231,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -406,11 +439,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="574134672"/>
-        <c:axId val="574135848"/>
+        <c:axId val="307063648"/>
+        <c:axId val="307064040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574134672"/>
+        <c:axId val="307063648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -452,7 +485,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574135848"/>
+        <c:crossAx val="307064040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -460,7 +493,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574135848"/>
+        <c:axId val="307064040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,7 +543,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574134672"/>
+        <c:crossAx val="307063648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -784,11 +817,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565786104"/>
-        <c:axId val="565786496"/>
+        <c:axId val="311156352"/>
+        <c:axId val="311156744"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565786104"/>
+        <c:axId val="311156352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +863,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565786496"/>
+        <c:crossAx val="311156744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,7 +871,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565786496"/>
+        <c:axId val="311156744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -888,7 +921,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565786104"/>
+        <c:crossAx val="311156352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -927,6 +960,470 @@
     </a:gradFill>
     <a:ln>
       <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>2000K Records</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2000K-MultipleSources'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (secs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2000K-MultipleSources'!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>73.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.808999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>130</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2000K-MultipleSources'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Memory Consumed(Mbs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2000K-MultipleSources'!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>189</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>283.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>420</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'2000K-MultipleSources'!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No of Sources</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'2000K-MultipleSources'!$D$2:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="522294344"/>
+        <c:axId val="522295520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="522294344"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522295520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="522295520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="522294344"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
     </a:ln>
     <a:effectLst/>
   </c:spPr>
@@ -1191,11 +1688,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="574138592"/>
-        <c:axId val="574136240"/>
+        <c:axId val="307064824"/>
+        <c:axId val="307065216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574138592"/>
+        <c:axId val="307064824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1734,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574136240"/>
+        <c:crossAx val="307065216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1245,7 +1742,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574136240"/>
+        <c:axId val="307065216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,7 +1792,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574138592"/>
+        <c:crossAx val="307064824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1625,11 +2122,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="566698392"/>
-        <c:axId val="566697608"/>
+        <c:axId val="307066000"/>
+        <c:axId val="307066392"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="566698392"/>
+        <c:axId val="307066000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1671,7 +2168,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="566697608"/>
+        <c:crossAx val="307066392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1679,7 +2176,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="566697608"/>
+        <c:axId val="307066392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +2226,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="566698392"/>
+        <c:crossAx val="307066000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2063,11 +2560,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="439113416"/>
-        <c:axId val="439111456"/>
+        <c:axId val="307067176"/>
+        <c:axId val="307067568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="439113416"/>
+        <c:axId val="307067176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2109,7 +2606,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439111456"/>
+        <c:crossAx val="307067568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2117,7 +2614,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="439111456"/>
+        <c:axId val="307067568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2167,7 +2664,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439113416"/>
+        <c:crossAx val="307067176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2578,11 +3075,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="574135456"/>
-        <c:axId val="574137416"/>
+        <c:axId val="307068352"/>
+        <c:axId val="312032928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574135456"/>
+        <c:axId val="307068352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2624,7 +3121,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574137416"/>
+        <c:crossAx val="312032928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2632,7 +3129,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574137416"/>
+        <c:axId val="312032928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2682,7 +3179,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574135456"/>
+        <c:crossAx val="307068352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2858,22 +3355,12 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="window" lastClr="FFFFFF">
                     <a:lumMod val="95000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:effectLst>
-                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
-                    <a:prstClr val="black">
-                      <a:alpha val="40000"/>
-                    </a:prstClr>
-                  </a:outerShdw>
-                </a:effectLst>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -3026,11 +3513,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="574138200"/>
-        <c:axId val="574135064"/>
+        <c:axId val="312033712"/>
+        <c:axId val="312034104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="574138200"/>
+        <c:axId val="312033712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3072,7 +3559,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574135064"/>
+        <c:crossAx val="312034104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3080,7 +3567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="574135064"/>
+        <c:axId val="312034104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3130,7 +3617,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="574138200"/>
+        <c:crossAx val="312033712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3584,11 +4071,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565788456"/>
-        <c:axId val="565784144"/>
+        <c:axId val="312034888"/>
+        <c:axId val="312035280"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565788456"/>
+        <c:axId val="312034888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3649,7 +4136,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565784144"/>
+        <c:crossAx val="312035280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3657,7 +4144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565784144"/>
+        <c:axId val="312035280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3718,7 +4205,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565788456"/>
+        <c:crossAx val="312034888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3879,15 +4366,12 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="window" lastClr="FFFFFF">
                     <a:lumMod val="85000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
@@ -4027,11 +4511,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565782576"/>
-        <c:axId val="565787280"/>
+        <c:axId val="312036064"/>
+        <c:axId val="312036456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565782576"/>
+        <c:axId val="312036064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4092,7 +4576,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565787280"/>
+        <c:crossAx val="312036456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4100,7 +4584,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565787280"/>
+        <c:axId val="312036456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4161,7 +4645,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565782576"/>
+        <c:crossAx val="312036064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4690,11 +5174,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="565783752"/>
-        <c:axId val="565784928"/>
+        <c:axId val="311155176"/>
+        <c:axId val="311155568"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="565783752"/>
+        <c:axId val="311155176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4736,7 +5220,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565784928"/>
+        <c:crossAx val="311155568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4744,7 +5228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="565784928"/>
+        <c:axId val="311155568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4794,7 +5278,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="565783752"/>
+        <c:crossAx val="311155176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4926,6 +5410,46 @@
 </file>
 
 <file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6277,6 +6801,555 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="236">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="233">
   <cs:axisTitle>
@@ -10684,280 +11757,39 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="1 StreamingSource (2)"/>
-      <sheetName val="2 StreamingSources (2)"/>
-      <sheetName val="3 StreamingSources (2)"/>
-      <sheetName val="4 StreamingSources (2)"/>
-      <sheetName val="Parallel-5clients"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>Time (secs)</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>1K</v>
-          </cell>
-          <cell r="B6">
-            <v>0.36099999999999999</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>10K</v>
-          </cell>
-          <cell r="B7">
-            <v>1.226</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>100K</v>
-          </cell>
-          <cell r="B8">
-            <v>6.2210000000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>1000K</v>
-          </cell>
-          <cell r="B9">
-            <v>50.631999999999998</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>2000K</v>
-          </cell>
-          <cell r="B10">
-            <v>90.087000000000003</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="5">
-          <cell r="B5" t="str">
-            <v>SourceClient#1 - Time (secs)</v>
-          </cell>
-          <cell r="C5" t="str">
-            <v>SourceClient#2 - Time (secs)</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>1K</v>
-          </cell>
-          <cell r="B6">
-            <v>0.80700000000000005</v>
-          </cell>
-          <cell r="C6">
-            <v>0.56899999999999995</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>10K</v>
-          </cell>
-          <cell r="B7">
-            <v>1.639</v>
-          </cell>
-          <cell r="C7">
-            <v>1.657</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>100K</v>
-          </cell>
-          <cell r="B8">
-            <v>11.292999999999999</v>
-          </cell>
-          <cell r="C8">
-            <v>10.042999999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>1000K</v>
-          </cell>
-          <cell r="B9">
-            <v>65.018000000000001</v>
-          </cell>
-          <cell r="C9">
-            <v>62.526000000000003</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>2000K</v>
-          </cell>
-          <cell r="B10">
-            <v>238.101</v>
-          </cell>
-          <cell r="C10">
-            <v>232.12100000000001</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>1K</v>
-          </cell>
-          <cell r="B6">
-            <v>0.52</v>
-          </cell>
-          <cell r="C6">
-            <v>0.45600000000000002</v>
-          </cell>
-          <cell r="D6">
-            <v>0.498</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>10K</v>
-          </cell>
-          <cell r="B7">
-            <v>1.921</v>
-          </cell>
-          <cell r="C7">
-            <v>1.627</v>
-          </cell>
-          <cell r="D7">
-            <v>1.5660000000000001</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>100K</v>
-          </cell>
-          <cell r="B8">
-            <v>6.6390000000000002</v>
-          </cell>
-          <cell r="C8">
-            <v>6.468</v>
-          </cell>
-          <cell r="D8">
-            <v>6.4710000000000001</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>1000K</v>
-          </cell>
-          <cell r="B9">
-            <v>51.213999999999999</v>
-          </cell>
-          <cell r="C9">
-            <v>55.255000000000003</v>
-          </cell>
-          <cell r="D9">
-            <v>55.753</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>2000K</v>
-          </cell>
-          <cell r="B10">
-            <v>113.31399999999999</v>
-          </cell>
-          <cell r="C10">
-            <v>112.879</v>
-          </cell>
-          <cell r="D10">
-            <v>108.93</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="6">
-          <cell r="A6" t="str">
-            <v>1K</v>
-          </cell>
-          <cell r="B6">
-            <v>0.82899999999999996</v>
-          </cell>
-          <cell r="C6">
-            <v>0.64400000000000002</v>
-          </cell>
-          <cell r="D6">
-            <v>0.79600000000000004</v>
-          </cell>
-          <cell r="E6">
-            <v>0.57199999999999995</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7" t="str">
-            <v>10K</v>
-          </cell>
-          <cell r="B7">
-            <v>2.3290000000000002</v>
-          </cell>
-          <cell r="C7">
-            <v>2.2200000000000002</v>
-          </cell>
-          <cell r="D7">
-            <v>1.758</v>
-          </cell>
-          <cell r="E7">
-            <v>1.748</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8" t="str">
-            <v>100K</v>
-          </cell>
-          <cell r="B8">
-            <v>7.8869999999999996</v>
-          </cell>
-          <cell r="C8">
-            <v>7.944</v>
-          </cell>
-          <cell r="D8">
-            <v>7.4530000000000003</v>
-          </cell>
-          <cell r="E8">
-            <v>8.0860000000000003</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9" t="str">
-            <v>1000K</v>
-          </cell>
-          <cell r="B9">
-            <v>63.945999999999998</v>
-          </cell>
-          <cell r="C9">
-            <v>63.691000000000003</v>
-          </cell>
-          <cell r="D9">
-            <v>62.438000000000002</v>
-          </cell>
-          <cell r="E9">
-            <v>69.629000000000005</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="A10" t="str">
-            <v>2000K</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>981075</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11225,8 +12057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11558,7 +12390,7 @@
   <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11980,8 +12812,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12494,8 +13326,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12847,7 +13679,7 @@
         <v>61.643333333333338</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:F21" si="3">AVERAGE(C18:C20)</f>
+        <f t="shared" ref="C21:E21" si="3">AVERAGE(C18:C20)</f>
         <v>65.042333333333332</v>
       </c>
       <c r="D21" s="7">
@@ -13074,8 +13906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13656,4 +14488,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>73.63</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1">
+        <v>97.808999999999997</v>
+      </c>
+      <c r="C3" s="1">
+        <v>189</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1">
+        <v>110</v>
+      </c>
+      <c r="C4" s="1">
+        <v>283.33</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1">
+        <v>130</v>
+      </c>
+      <c r="C5" s="1">
+        <v>420</v>
+      </c>
+      <c r="D5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>